<commit_message>
Atualiza planilhas mensais (run 2025-09-15)
</commit_message>
<xml_diff>
--- a/data/erros_carrefour_2025-09.xlsx
+++ b/data/erros_carrefour_2025-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1075,6 +1075,626 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Páprica Defumada Kitano Reserva 36g</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farofa-de-mandioca-tradicional-yoki-400g-6582613/p</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/massa-para-pastel-discao-massa-leve-500g-841757/p</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Pimentão Block Vermelho Trebeshi 150 g</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/pimentao-block-vermelho-trebeshi-150-g-5738458/p</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/chocolate-ao-leite-com-amendoim-shot-165g-5790859/p</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Laranja Pera Carrefour Mercado 5 Kg</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/laranja-pera-carrefour-mercado-5-kg-6282032/p</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/patinho-fracionado-a-vacuo-500g-18325/p</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/paleta-bovina-a-vacuo-500gnao-reativarcodigo-de-compra-20745/p</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/costela-minga-bovina-cong-aprox-2kg-224006/p</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/presunto-cozido-sem-capa-fatiado-aurora-aproximadamente-200-g-49450/p</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mortadela-defumada-sadia-280g-5447045/p</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-minas-frescal-aurora-450-g-6264693/p</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-coalho-bom-leite-500-g-4305054/p</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/leite-uht-integral-piratininga-1-l-665017/p</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/iogurte-natural-tradicional-batavo-170g-5150439/p</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/manteiga-com-sal-aviacao-200-g-10010/p</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/creme-de-leite-ultrapasteurizado-itambe-200-g-5988921/p</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/requeijao-cremoso-aviacao-tradicional-220-g-10000/p</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/acucar-cristal-carrefour-1kg-5147300/p</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mel-com-cacau-e-avela-400-g-4510146/p</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/geleia-de-goiaba-selecoes-c-pedacos-260-g-1280815/p</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/suco-de-uva-integral-maric-1-l-3538256/p</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/vinho-tinto-fino-seco-cabernet-sauvignon-pergola-750ml-1521709/p</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/whisky-red-label-johnnie-walker-1-litro-2719/p</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/refrigerante-coca-cola-sabor-cola-1-5-l-11087/p</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/cafe-torrado-e-moido-extraforte-melitta-500g-271203/p</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farinha-de-trigo-dona-benta-tradicional-1kg-196416/p</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/azeite-extravirgem-portugues-oliveira-da-serra-500-ml-4526108/p</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/oleo-de-soja-soya-900ml-482616/p</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/margarina-qualy-com-sal-250g-4815618/p</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/arroz-branco-longofino-tipo-1-tio-joao-1kg-115658/p</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/feijao-preto-tipo-1-kicaldo-1kg-466510/p</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualiza planilhas mensais (run 2025-09-16)
</commit_message>
<xml_diff>
--- a/data/erros_carrefour_2025-09.xlsx
+++ b/data/erros_carrefour_2025-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,6 +1695,606 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Páprica Defumada Kitano Reserva 36g</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farofa-de-mandioca-tradicional-yoki-400g-6582613/p</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/massa-para-pastel-discao-massa-leve-500g-841757/p</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Pimentão Block Vermelho Trebeshi 150 g</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/pimentao-block-vermelho-trebeshi-150-g-5738458/p</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/chocolate-ao-leite-com-amendoim-shot-165g-5790859/p</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/patinho-fracionado-a-vacuo-500g-18325/p</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/paleta-bovina-a-vacuo-500gnao-reativarcodigo-de-compra-20745/p</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/costela-minga-bovina-cong-aprox-2kg-224006/p</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/presunto-cozido-sem-capa-fatiado-aurora-aproximadamente-200-g-49450/p</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mortadela-defumada-sadia-280g-5447045/p</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-minas-frescal-aurora-450-g-6264693/p</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-coalho-bom-leite-500-g-4305054/p</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/leite-uht-integral-piratininga-1-l-665017/p</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/iogurte-natural-tradicional-batavo-170g-5150439/p</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/manteiga-com-sal-aviacao-200-g-10010/p</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/creme-de-leite-ultrapasteurizado-itambe-200-g-5988921/p</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/requeijao-cremoso-aviacao-tradicional-220-g-10000/p</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/acucar-cristal-carrefour-1kg-5147300/p</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mel-com-cacau-e-avela-400-g-4510146/p</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/geleia-de-goiaba-selecoes-c-pedacos-260-g-1280815/p</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/suco-de-uva-integral-maric-1-l-3538256/p</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/vinho-tinto-fino-seco-cabernet-sauvignon-pergola-750ml-1521709/p</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/whisky-red-label-johnnie-walker-1-litro-2719/p</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/refrigerante-coca-cola-sabor-cola-1-5-l-11087/p</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/cafe-torrado-e-moido-extraforte-melitta-500g-271203/p</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farinha-de-trigo-dona-benta-tradicional-1kg-196416/p</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/azeite-extravirgem-portugues-oliveira-da-serra-500-ml-4526108/p</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/oleo-de-soja-soya-900ml-482616/p</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/margarina-qualy-com-sal-250g-4815618/p</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/arroz-branco-longofino-tipo-1-tio-joao-1kg-115658/p</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/feijao-preto-tipo-1-kicaldo-1kg-466510/p</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualiza planilhas mensais (run 2025-09-18)
</commit_message>
<xml_diff>
--- a/data/erros_carrefour_2025-09.xlsx
+++ b/data/erros_carrefour_2025-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3135,6 +3135,846 @@
         </is>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Páprica Defumada Kitano Reserva 36g</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farofa-de-mandioca-tradicional-yoki-400g-6582613/p</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/massa-para-pastel-discao-massa-leve-500g-841757/p</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Pimentão Block Vermelho Trebeshi 150 g</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/pimentao-block-vermelho-trebeshi-150-g-5738458/p</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/chocolate-ao-leite-com-amendoim-shot-165g-5790859/p</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Couve Flor Cledson 300 g</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/couve-flor-cledson-300-g-9560297/p</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>0</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/patinho-fracionado-a-vacuo-500g-18325/p</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/paleta-bovina-a-vacuo-500gnao-reativarcodigo-de-compra-20745/p</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/costela-minga-bovina-cong-aprox-2kg-224006/p</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/presunto-cozido-sem-capa-fatiado-aurora-aproximadamente-200-g-49450/p</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mortadela-defumada-sadia-280g-5447045/p</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-minas-frescal-aurora-450-g-6264693/p</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>0</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/queijo-coalho-bom-leite-500-g-4305054/p</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/leite-uht-integral-piratininga-1-l-665017/p</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/iogurte-natural-tradicional-batavo-170g-5150439/p</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/manteiga-com-sal-aviacao-200-g-10010/p</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/creme-de-leite-ultrapasteurizado-itambe-200-g-5988921/p</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/requeijao-cremoso-aviacao-tradicional-220-g-10000/p</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/acucar-cristal-carrefour-1kg-5147300/p</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/mel-com-cacau-e-avela-400-g-4510146/p</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/geleia-de-goiaba-selecoes-c-pedacos-260-g-1280815/p</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/suco-de-uva-integral-maric-1-l-3538256/p</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/vinho-tinto-fino-seco-cabernet-sauvignon-pergola-750ml-1521709/p</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/whisky-red-label-johnnie-walker-1-litro-2719/p</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/refrigerante-coca-cola-sabor-cola-1-5-l-11087/p</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/cafe-torrado-e-moido-extraforte-melitta-500g-271203/p</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/farinha-de-trigo-dona-benta-tradicional-1kg-196416/p</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/azeite-extravirgem-portugues-oliveira-da-serra-500-ml-4526108/p</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/oleo-de-soja-soya-900ml-482616/p</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/margarina-qualy-com-sal-250g-4815618/p</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/arroz-branco-longofino-tipo-1-tio-joao-1kg-115658/p</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/feijao-preto-tipo-1-kicaldo-1kg-466510/p</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Arroz Branco Carrefour Classic Olimpíadas 1Kg</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/arroz-branco-carrefour-classic-olimpiadas-1kg-3433455/p</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/pao%20frances</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/biscoito%20doce</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/frango-inteiro-temperado-seara-assa-facil-aprox-19kg-170739/p</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/cafe%20moido</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/costela?page=1</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/costela-de-cordeiro-a-vacuo-28738/p</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/lingui%C3%A7a</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>0</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/busca/lingui%C3%A7a?page=3</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Ovo Branco Grande Mantiqueira Happy Eggs com 20 Unidades</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/ovo-branco-grande-mantiqueira-happy-eggs-com-20-unidades-6403565/p</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Óleo de Soja Confiare 900ml</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>0</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://mercado.carrefour.com.br/oleo-de-soja-confiare-900ml-3731243/p</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>